<commit_message>
Added links for examples
</commit_message>
<xml_diff>
--- a/Datasets links.xlsx
+++ b/Datasets links.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaacjohnson/Documents/Scanner Output/School/Willamette/Capstone/Capstone Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse\Documents\Schooling\Willamette-MSDS\2-DATA510_Capstone\MSDS-Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46376AA-FF5F-AB44-BFB6-892E3884FEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93023D7-7237-41E2-A00B-FA1A1EB75F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{1F35278B-75FA-2D41-B65E-A2FD34DFEB03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F35278B-75FA-2D41-B65E-A2FD34DFEB03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>https://www.google.com/search?client=safari&amp;rls=en&amp;q=incidence+rates+of+diabetes+per+county&amp;ie=UTF-8&amp;oe=UTF-8</t>
   </si>
@@ -156,6 +156,39 @@
   </si>
   <si>
     <t>https://www.census.gov/data/developers/data-sets.html</t>
+  </si>
+  <si>
+    <t>https://jscholarship.library.jhu.edu/bitstream/handle/1774.2/61821/Wallace,%20Robyn.pdf?sequence=1</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/36276352/</t>
+  </si>
+  <si>
+    <t>https://digitalcommons.csumb.edu/cgi/viewcontent.cgi?article=1849&amp;context=caps_thes_all</t>
+  </si>
+  <si>
+    <t>https://scholarworks.gsu.edu/cgi/viewcontent.cgi?article=1022&amp;context=iph_capstone</t>
+  </si>
+  <si>
+    <t>Example capstones, reports, articles, etc.</t>
+  </si>
+  <si>
+    <t>https://www.brookings.edu/blog/usc-brookings-schaeffer-on-health-policy/2020/02/19/there-are-clear-race-based-inequalities-in-health-insurance-and-health-outcomes/</t>
+  </si>
+  <si>
+    <t>https://www.kff.org/racial-equity-and-health-policy/report/key-data-on-health-and-health-care-by-race-and-ethnicity/</t>
+  </si>
+  <si>
+    <t>https://www.kff.org/report-section/key-data-on-health-and-health-care-by-race-ethnicity-methodology/</t>
+  </si>
+  <si>
+    <t>https://data.census.gov/table</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/datasets/utkarshxy/who-worldhealth-statistics-2020-complete</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/code/noobiedatascientist/explaining-happiness</t>
   </si>
 </sst>
 </file>
@@ -518,19 +551,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B7320E-AD74-1C46-9EC5-2B89B3B8451E}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="32.69921875" customWidth="1"/>
+    <col min="2" max="2" width="29.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -538,12 +571,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -562,7 +595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -570,7 +603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -578,7 +611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -586,10 +619,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -597,17 +630,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -615,7 +648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -623,7 +656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -631,7 +664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -639,7 +672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -647,7 +680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -655,7 +688,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -663,44 +696,105 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -726,6 +820,16 @@
     <hyperlink ref="A29" r:id="rId19" xr:uid="{3E94B8D8-7983-5042-9C8C-5FE56E978919}"/>
     <hyperlink ref="A30" r:id="rId20" xr:uid="{20FAC450-40F1-194E-98CC-F0F446F6DDF5}"/>
     <hyperlink ref="A31" r:id="rId21" xr:uid="{9A731716-E361-2D4A-959B-334E53585DDB}"/>
+    <hyperlink ref="A38" r:id="rId22" xr:uid="{43732DBC-4D0A-4933-98BC-90EFB72CD9BD}"/>
+    <hyperlink ref="A39" r:id="rId23" xr:uid="{13CECEDB-4953-4710-8974-34F0A26BFAB5}"/>
+    <hyperlink ref="A40" r:id="rId24" xr:uid="{1440E0A7-D4D5-4A70-8BB5-A1357369EBA2}"/>
+    <hyperlink ref="A41" r:id="rId25" xr:uid="{BAF570C6-D099-4426-98A2-8AA55084D66C}"/>
+    <hyperlink ref="A42" r:id="rId26" xr:uid="{9E43A04B-471B-464F-A64E-756B7CAD9332}"/>
+    <hyperlink ref="A43" r:id="rId27" xr:uid="{1DF00B65-AB16-4EDA-8578-264457C6CFA4}"/>
+    <hyperlink ref="A44" r:id="rId28" xr:uid="{516AE935-AE45-4C85-AD28-AFB7963F0E78}"/>
+    <hyperlink ref="A32" r:id="rId29" xr:uid="{D8EAAB6A-99C4-4034-80D5-2F32711598B8}"/>
+    <hyperlink ref="A33" r:id="rId30" xr:uid="{3D94759D-6230-4646-B5DB-B7B44EB7E71A}"/>
+    <hyperlink ref="A45" r:id="rId31" xr:uid="{D57DBF4C-D5A7-435C-8858-5960530EDAE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>